<commit_message>
Added absorb and reflect elemental damages, changed lightning to bolt, added ICaster interface, made stagger count down instead of up
Added absorb and reflect special elemental resistances (constants -1 and -2 respectively) and implemented their effects for single taget spells. changed lighnint element to bolt (its easier to type) added ICaster interface wich enemy and Player implement to simplify spellcasting code. may make more polymorphic refinements with a Casterstats base class to later clean up casting code
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/enemyDatabase.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rockpolotics\unity_projects\GDA\typocrypha\Typocrypha\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enemyDatabase" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>ice wk/res</t>
   </si>
   <si>
-    <t>lightning wk/res</t>
-  </si>
-  <si>
     <t>Spell1 (root)</t>
   </si>
   <si>
@@ -112,12 +109,15 @@
   </si>
   <si>
     <t>poke</t>
+  </si>
+  <si>
+    <t>bolt wk/res</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -951,37 +951,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" customWidth="1"/>
-    <col min="17" max="17" width="10.28515625" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" customWidth="1"/>
     <col min="19" max="19" width="10" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -990,7 +990,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1017,33 +1017,33 @@
         <v>10</v>
       </c>
       <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1082,33 +1082,33 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T2" t="s">
-        <v>20</v>
-      </c>
-      <c r="U2" t="s">
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -1147,24 +1147,24 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="P3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>20</v>
-      </c>
-      <c r="R3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>50</v>
@@ -1191,7 +1191,7 @@
         <v>5</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L4">
         <v>2</v>
@@ -1200,33 +1200,33 @@
         <v>0.75</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="O4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" t="s">
         <v>19</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" t="s">
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>20</v>
-      </c>
-      <c r="R4" t="s">
-        <v>23</v>
-      </c>
-      <c r="S4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>